<commit_message>
mergelist script will replace themes when encountering unexpected duplicates
</commit_message>
<xml_diff>
--- a/tests/data/scifi1920-mergelist.xlsx
+++ b/tests/data/scifi1920-mergelist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
   <si>
     <t xml:space="preserve">sid</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t xml:space="preserve">delete for missing theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Obal and Peter Hell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mother and son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">different capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insert new theme though it is already present</t>
   </si>
 </sst>
 </file>
@@ -142,7 +154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -172,13 +184,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -275,11 +280,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,6 +290,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -556,12 +561,12 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M5" activeCellId="0" sqref="M5"/>
+      <selection pane="bottomRight" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="70" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -604,7 +609,7 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -645,14 +650,14 @@
       <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5"/>
+      <c r="H2" s="4"/>
       <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="7"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="70" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -673,7 +678,7 @@
       <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="4"/>
       <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
@@ -686,7 +691,7 @@
       <c r="L3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="7"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="70" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -707,10 +712,10 @@
       <c r="G4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="7"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -751,7 +756,7 @@
       <c r="G6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -774,10 +779,37 @@
       <c r="G7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -865,7 +897,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="59.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="7" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="70" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -928,28 +960,28 @@
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="7"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="70" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G3" s="5"/>
-      <c r="M3" s="7"/>
+      <c r="G3" s="4"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="70" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G4" s="5"/>
-      <c r="M4" s="7"/>
+      <c r="G4" s="4"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="5"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G4 G6:G7">
@@ -983,7 +1015,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F87" activeCellId="0" sqref="F87"/>
     </sheetView>
   </sheetViews>

</xml_diff>